<commit_message>
Initial Sprint 2 Burn Up Chart
</commit_message>
<xml_diff>
--- a/info/Burn Up Chart.xlsx
+++ b/info/Burn Up Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\School\CMPS 115\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\GitHub\CMPS115-Project\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -205,15 +205,6 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -265,16 +256,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,11 +280,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333068504"/>
-        <c:axId val="333066152"/>
+        <c:axId val="330757624"/>
+        <c:axId val="330757232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333068504"/>
+        <c:axId val="330757624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,12 +341,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333066152"/>
+        <c:crossAx val="330757232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333066152"/>
+        <c:axId val="330757232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,7 +463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333068504"/>
+        <c:crossAx val="330757624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1410,7 +1401,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1413,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -1436,35 +1427,26 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>3</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Burn Up Chart for Sprint 2
</commit_message>
<xml_diff>
--- a/info/Burn Up Chart.xlsx
+++ b/info/Burn Up Chart.xlsx
@@ -177,10 +177,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:f>Sheet1!$C$1:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -192,18 +192,33 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$4</c:f>
+              <c:f>Sheet1!$D$1:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -230,10 +245,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:f>Sheet1!$C$1:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -245,16 +260,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Sheet1!$B$1:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>47</c:v>
                 </c:pt>
@@ -265,6 +283,9 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
@@ -280,11 +301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330757624"/>
-        <c:axId val="330757232"/>
+        <c:axId val="246673472"/>
+        <c:axId val="246708752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330757624"/>
+        <c:axId val="246673472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,12 +362,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330757232"/>
+        <c:crossAx val="246708752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330757232"/>
+        <c:axId val="246708752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,7 +484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330757624"/>
+        <c:crossAx val="246673472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1398,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,6 +1453,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -1440,6 +1464,9 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -1447,6 +1474,20 @@
       </c>
       <c r="C4">
         <v>3</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>